<commit_message>
Modified version (email detail)
</commit_message>
<xml_diff>
--- a/EmailDetails.xlsx
+++ b/EmailDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liou\Documents\UiPath\UiPath-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B350D53-51AC-44C7-8A43-C92DC3425968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D3BB0B-1E96-44AA-A1B5-13D5C7E3BE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="380" windowWidth="15670" windowHeight="9700" xr2:uid="{DED59434-A757-4FCD-8EF5-3BE5A6613702}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DED59434-A757-4FCD-8EF5-3BE5A6613702}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>EmailType</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>melvinngweixiang@gmail.com,2101000d@student.tp.edu.sg</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Testing4</t>
+  </si>
+  <si>
+    <t>Testing3</t>
   </si>
 </sst>
 </file>
@@ -432,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F099D4-DB81-45D5-812F-206597ED80E3}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,11 +520,58 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D3A27F48-78D9-4720-9A02-09EE564D7A17}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{759B95F8-1D7E-49E8-B8C1-73481FCDA99B}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{9DD75D30-EC06-46EA-979D-D8273093C725}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{6D29A70C-5E1C-4DAB-92DE-03A5CEDC61D9}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{B37F5D15-5354-4ED1-AA49-F4B176D7825B}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{671A9AFD-4A89-44BF-8A9E-D0C0ADC676AD}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{F57F426A-F366-450C-A772-001F3F1CA83F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>